<commit_message>
add -g command line option.
</commit_message>
<xml_diff>
--- a/csharp2/results.xlsx
+++ b/csharp2/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\clovett\primes\csharp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B7709E-5921-444E-A377-C963A535D729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA184652-8C61-45D0-A3CE-1CD686FE4824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1755" yWindow="2145" windowWidth="25110" windowHeight="14385" xr2:uid="{AF12124C-4EFC-4AA6-B744-AB748D3A4AB0}"/>
   </bookViews>
@@ -1488,7 +1488,7 @@
   <dimension ref="C2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1529,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <f>D4/D3</f>
+        <f t="shared" ref="E4:E9" si="0">D4/D3</f>
         <v>2</v>
       </c>
       <c r="F4">
@@ -1544,7 +1544,7 @@
         <v>13</v>
       </c>
       <c r="E5">
-        <f>D5/D4</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="F5">
@@ -1559,7 +1559,7 @@
         <v>195</v>
       </c>
       <c r="E6">
-        <f>D6/D5</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F6">
@@ -1574,7 +1574,7 @@
         <v>2508</v>
       </c>
       <c r="E7">
-        <f>D7/D6</f>
+        <f t="shared" si="0"/>
         <v>12.861538461538462</v>
       </c>
       <c r="F7">
@@ -1589,7 +1589,7 @@
         <v>32244</v>
       </c>
       <c r="E8">
-        <f>D8/D7</f>
+        <f t="shared" si="0"/>
         <v>12.85645933014354</v>
       </c>
       <c r="F8">
@@ -1605,7 +1605,7 @@
         <v>436176</v>
       </c>
       <c r="E9">
-        <f>D9/D8</f>
+        <f t="shared" si="0"/>
         <v>13.527353926311871</v>
       </c>
       <c r="F9">

</xml_diff>